<commit_message>
Added metric functionality and cleanup
</commit_message>
<xml_diff>
--- a/Research/results.xlsx
+++ b/Research/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rick\Documents\Git\Handwritten-digit-classification\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC47167-CCEB-4A37-A7A7-A7522F1E4B40}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76EA4F7B-7B13-4F02-9CB8-FB8FAC8F95A0}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17610" xr2:uid="{927AF142-C602-4221-AE13-F5EBDBB2685A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="18">
   <si>
     <t>Algorithm</t>
   </si>
@@ -69,60 +69,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>Metrics:</t>
-  </si>
-  <si>
-    <t>Classificatie</t>
-  </si>
-  <si>
-    <t>Mean absolute error</t>
-  </si>
-  <si>
-    <t>Median absolute deviation</t>
-  </si>
-  <si>
-    <t>Root mean squared error</t>
-  </si>
-  <si>
-    <t>R-Squared</t>
-  </si>
-  <si>
-    <t>Adjusted RMSE</t>
-  </si>
-  <si>
-    <t>Adjust R-Squared</t>
-  </si>
-  <si>
-    <t>Precision</t>
-  </si>
-  <si>
-    <t>Recall</t>
-  </si>
-  <si>
-    <t>Specificity</t>
-  </si>
-  <si>
-    <t>Kappa</t>
-  </si>
-  <si>
-    <t>AUC-ROC</t>
-  </si>
-  <si>
-    <t>AUC-PRC</t>
-  </si>
-  <si>
-    <t>F1-Score</t>
-  </si>
-  <si>
-    <t>Matthews correlation coefficient</t>
-  </si>
-  <si>
-    <t>Regression</t>
-  </si>
-  <si>
-    <t>Classification</t>
-  </si>
-  <si>
     <t>Pipeline results XGBoost</t>
   </si>
   <si>
@@ -130,6 +76,9 @@
   </si>
   <si>
     <t>Kaggle accuracy</t>
+  </si>
+  <si>
+    <t>0.00%</t>
   </si>
 </sst>
 </file>
@@ -1624,7 +1573,7 @@
   <dimension ref="A1:O56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1675,7 +1624,7 @@
         <v>1</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1703,7 +1652,7 @@
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1967,9 +1916,13 @@
       <c r="E16" s="3">
         <v>0.85799999999999998</v>
       </c>
-      <c r="J16" s="1"/>
+      <c r="J16" s="1">
+        <v>1</v>
+      </c>
       <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
+      <c r="L16" s="7">
+        <v>0.94971000000000005</v>
+      </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -2070,7 +2023,7 @@
         <v>1</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -2098,7 +2051,7 @@
         <v>1</v>
       </c>
       <c r="L24" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2191,7 +2144,9 @@
       <c r="J28" s="1">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="K28" s="3"/>
+      <c r="K28" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -2268,7 +2223,9 @@
       <c r="K31" s="7">
         <v>0.96899999999999997</v>
       </c>
-      <c r="L31" s="7"/>
+      <c r="L31" s="7">
+        <v>0.96699999999999997</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -2294,9 +2251,11 @@
       <c r="K32" s="8">
         <v>0.97360000000000002</v>
       </c>
-      <c r="L32" s="8"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L32" s="8">
+        <v>0.97199999999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -2317,14 +2276,11 @@
       <c r="J33" s="1">
         <v>0.8</v>
       </c>
-      <c r="K33" s="8">
-        <v>0.97899999999999998</v>
-      </c>
       <c r="L33" s="8">
-        <v>0.97899999999999998</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.97699999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -2342,8 +2298,14 @@
       <c r="E34" s="3">
         <v>0.83</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J34" s="8">
+        <v>1</v>
+      </c>
+      <c r="L34" s="8">
+        <v>0.97899999999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -2361,8 +2323,9 @@
       <c r="E35" s="3">
         <v>0.92</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J35" s="8"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -2381,7 +2344,7 @@
         <v>0.92589999999999995</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -2400,7 +2363,7 @@
         <v>0.93100000000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>9</v>
       </c>
@@ -2419,12 +2382,12 @@
         <v>0.93300000000000005</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -2443,11 +2406,8 @@
       <c r="F41" t="s">
         <v>12</v>
       </c>
-      <c r="K41" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>2</v>
       </c>
@@ -2469,7 +2429,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>2</v>
       </c>
@@ -2490,17 +2450,10 @@
       <c r="F43" s="7">
         <v>0.93569999999999998</v>
       </c>
-      <c r="K43" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="L43" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="M43" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K43" s="6"/>
+      <c r="L43" s="6"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>2</v>
       </c>
@@ -2522,17 +2475,8 @@
         <v>0.93569999999999998</v>
       </c>
       <c r="G44" s="7"/>
-      <c r="K44" t="s">
-        <v>16</v>
-      </c>
-      <c r="L44" t="s">
-        <v>1</v>
-      </c>
-      <c r="M44" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>2</v>
       </c>
@@ -2554,17 +2498,8 @@
         <v>0.93569999999999998</v>
       </c>
       <c r="G45" s="7"/>
-      <c r="K45" t="s">
-        <v>17</v>
-      </c>
-      <c r="L45" t="s">
-        <v>22</v>
-      </c>
-      <c r="M45" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>2</v>
       </c>
@@ -2585,100 +2520,46 @@
         <v>0.94971000000000005</v>
       </c>
       <c r="G46" s="8"/>
-      <c r="K46" t="s">
-        <v>18</v>
-      </c>
-      <c r="L46" t="s">
-        <v>23</v>
-      </c>
-      <c r="M46" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="E47" s="3"/>
       <c r="G47" s="8"/>
-      <c r="K47" t="s">
-        <v>20</v>
-      </c>
-      <c r="L47" t="s">
-        <v>24</v>
-      </c>
-      <c r="M47" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
       <c r="E48" s="3"/>
       <c r="G48" s="7"/>
-      <c r="K48" t="s">
-        <v>19</v>
-      </c>
-      <c r="L48" t="s">
-        <v>25</v>
-      </c>
-      <c r="M48" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="E49" s="3"/>
-      <c r="K49" t="s">
-        <v>21</v>
-      </c>
-      <c r="L49" t="s">
-        <v>26</v>
-      </c>
-      <c r="M49" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="E50" s="3"/>
-      <c r="L50" t="s">
-        <v>27</v>
-      </c>
-      <c r="M50" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="E51" s="3"/>
-      <c r="L51" t="s">
-        <v>28</v>
-      </c>
-      <c r="M51" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="E52" s="3"/>
-      <c r="L52" t="s">
-        <v>29</v>
-      </c>
-      <c r="M52" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
       <c r="E53" s="3"/>
     </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
       <c r="E54" s="3"/>
     </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
       <c r="E55" s="5"/>
     </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
       <c r="E56" s="5"/>
     </row>

</xml_diff>